<commit_message>
habe mal ein test-kommentar in Ispieldaten geschrieben
</commit_message>
<xml_diff>
--- a/Dokumente/02_Arbeitsbereich/04_Anforderungsspezifikation/Dialogbeschreibungen/Dialogbeschreibung_Popup_Würfeln_Verteidiger.xlsx
+++ b/Dokumente/02_Arbeitsbereich/04_Anforderungsspezifikation/Dialogbeschreibungen/Dialogbeschreibung_Popup_Würfeln_Verteidiger.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robinlauenroth/Documents/SE-Project2018/Dokumente/02_Arbeitsbereich/04_Anforderungsspezifikation/Dialogbeschreibungen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F93CF60-39CA-DD43-86EB-31FC94ACFDD8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1C86CB-CDE5-F74E-A883-5087D6C4782C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,7 +96,7 @@
     <t>Bild mit Augenzahl der Würfel (max. 2 Würfel)</t>
   </si>
   <si>
-    <t>leer bevpr gewürfelt wurde</t>
+    <t>leer bevor gewürfelt wurde</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>